<commit_message>
Update sugar kelp example
</commit_message>
<xml_diff>
--- a/examples/sugar kelp/traits.xlsx
+++ b/examples/sugar kelp/traits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/djw64/OneDrive - Cornell University/T3/projects/ontology scripts/examples/sugar kelp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/djw64/Google Drive/Cornell/T3/projects/Trait Ontologies/ontology-scripts/examples/sugar kelp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EAE284-50F2-3940-A584-97C654B2260A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D50BE6-2A0C-CE42-840A-B8FF8869304F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6500" yWindow="3080" windowWidth="33580" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18440" yWindow="780" windowWidth="42920" windowHeight="26840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,19 @@
     <sheet name="Trait Classes" sheetId="5" r:id="rId5"/>
     <sheet name="Root" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1913,8 +1922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1922,15 +1931,15 @@
     <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="30" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" style="5" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="7" max="7" width="30" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" customWidth="1"/>
+    <col min="10" max="10" width="15.5" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="5" customWidth="1"/>
     <col min="15" max="15" width="19" customWidth="1"/>
     <col min="16" max="16" width="38.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.5" bestFit="1" customWidth="1"/>

</xml_diff>